<commit_message>
recherche des donnees pour 3 nouvelles variables
</commit_message>
<xml_diff>
--- a/Jeux de DD propre.xlsx
+++ b/Jeux de DD propre.xlsx
@@ -5,35 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours\MIASHS\Maraton-du-web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thach\OneDrive\Documents\M1 MIASHS\Marathon du web\Maraton-du-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81F5750-07BD-42FB-A12D-3A6EB50540FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B542A14D-BD21-474E-9825-F78FAA19C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27015" yWindow="2400" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Réponses au formulaire 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
   <si>
     <t>Nom de votre collectivité</t>
   </si>
@@ -265,6 +252,54 @@
   </si>
   <si>
     <t>Moyen +</t>
+  </si>
+  <si>
+    <t>171 habitants au km2</t>
+  </si>
+  <si>
+    <t>péri-urbain et semi-rural.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Auvergne-Rhône-Alpes </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 257 habitats au km2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> péri-urbain et semi-rural. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bretagne </t>
+  </si>
+  <si>
+    <t>76 habitats au km2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> péri-urbain,semi-rural et rural </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grand Est </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 262 habitatsau km2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> péri-urbain </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pays de la Loire </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1303 habitats au km2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> urbain et péri-urbain </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 129 habitats au km2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> urbain à rural </t>
   </si>
 </sst>
 </file>
@@ -359,7 +394,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -579,23 +614,23 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomRight" activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="51.5703125" customWidth="1"/>
-    <col min="6" max="23" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7265625" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" customWidth="1"/>
+    <col min="4" max="4" width="29.453125" customWidth="1"/>
+    <col min="5" max="5" width="51.54296875" customWidth="1"/>
+    <col min="6" max="23" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -648,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>45001.677176620375</v>
       </c>
@@ -685,15 +720,20 @@
       <c r="L2" s="3">
         <v>102.79</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>45001.729072118054</v>
       </c>
@@ -730,15 +770,20 @@
       <c r="L3" s="3">
         <v>103.8</v>
       </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="Q3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>45002.416117141205</v>
       </c>
@@ -775,12 +820,17 @@
       <c r="L4" s="3">
         <v>81</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>45002.449634259261</v>
       </c>
@@ -817,15 +867,20 @@
       <c r="L5" s="3">
         <v>91</v>
       </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="M5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="Q5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>45002.627384050924</v>
       </c>
@@ -862,15 +917,20 @@
       <c r="L6" s="3">
         <v>96</v>
       </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="M6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="Q6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>45002.650517083333</v>
       </c>
@@ -907,15 +967,20 @@
       <c r="L7" s="3">
         <v>86</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="M7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="Q7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>45005.564700925926</v>
       </c>
@@ -957,7 +1022,7 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>45005.621300856481</v>
       </c>
@@ -999,7 +1064,7 @@
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>45005.631334247686</v>
       </c>
@@ -1044,7 +1109,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>45007.493851562496</v>
       </c>
@@ -1089,7 +1154,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>45008.446508553243</v>
       </c>
@@ -1134,7 +1199,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>45014.472854074076</v>
       </c>
@@ -1179,7 +1244,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>45015.485319687505</v>
       </c>
@@ -1221,7 +1286,7 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>45015.494416099536</v>
       </c>
@@ -1271,7 +1336,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>45015.675072337966</v>
       </c>
@@ -1324,7 +1389,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>45015.679077731482</v>
       </c>
@@ -1377,7 +1442,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>45015.703346759256</v>
       </c>
@@ -1427,7 +1492,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>45016.342198321756</v>
       </c>
@@ -1480,7 +1545,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>45016.42414427083</v>
       </c>
@@ -1533,7 +1598,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>45016.51286357639</v>
       </c>
@@ -1586,7 +1651,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>45016.690710104165</v>
       </c>

</xml_diff>

<commit_message>
coor des collectivite rouge
</commit_message>
<xml_diff>
--- a/Jeux de DD propre.xlsx
+++ b/Jeux de DD propre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thach\OneDrive\Documents\M1 MIASHS\Marathon du web\Maraton-du-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E55EDE4-EA2A-4455-B249-0A066D0368B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49452F8-C86C-4906-9B4E-E1B711DF2A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Réponses au formulaire 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="103">
   <si>
     <t>Nom de votre collectivité</t>
   </si>
@@ -263,46 +263,73 @@
     <t xml:space="preserve"> 257 habitats au km2 </t>
   </si>
   <si>
-    <t xml:space="preserve"> péri-urbain et semi-rural. </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Bretagne </t>
   </si>
   <si>
     <t>76 habitats au km2</t>
   </si>
   <si>
-    <t xml:space="preserve"> péri-urbain,semi-rural et rural </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Grand Est </t>
   </si>
   <si>
     <t xml:space="preserve"> 262 habitatsau km2 </t>
   </si>
   <si>
-    <t xml:space="preserve"> péri-urbain </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Pays de la Loire </t>
   </si>
   <si>
     <t xml:space="preserve"> 1303 habitats au km2 </t>
   </si>
   <si>
-    <t xml:space="preserve"> urbain et péri-urbain </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 129 habitats au km2 </t>
   </si>
   <si>
-    <t xml:space="preserve"> urbain à rural </t>
-  </si>
-  <si>
     <t>peu dense</t>
   </si>
   <si>
     <t>Coordonnées</t>
+  </si>
+  <si>
+    <t>44° 46′ 13″ nord, 0° 18′ 38″ ouest</t>
+  </si>
+  <si>
+    <t>Isère</t>
+  </si>
+  <si>
+    <t>45° 21′ 51″ nord, 5° 35′ 26″ est</t>
+  </si>
+  <si>
+    <t>Ille-et-Vilaine</t>
+  </si>
+  <si>
+    <t>47° 52′ 41″ nord, 1° 47′ 14″ ouest</t>
+  </si>
+  <si>
+    <t>Meurthe-et-Moselle</t>
+  </si>
+  <si>
+    <t>densité intermédiaire</t>
+  </si>
+  <si>
+    <t>48° 46′ 08″ nord, 6° 07′ 42″ est</t>
+  </si>
+  <si>
+    <t>Loire-Atlantique</t>
+  </si>
+  <si>
+    <t>densement peuplé</t>
+  </si>
+  <si>
+    <t>47° 13′ 05″ nord, 1° 33′ 10″ ouest</t>
+  </si>
+  <si>
+    <t>Bas-Rhin, Haut-Rhin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">densité intermédiaire </t>
+  </si>
+  <si>
+    <t>48° 19′ 29″ nord, 7° 25′ 41″ est</t>
   </si>
 </sst>
 </file>
@@ -312,7 +339,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -340,8 +367,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,8 +400,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -375,12 +415,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -395,9 +451,14 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -617,10 +678,10 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q4" sqref="Q4"/>
+      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -683,13 +744,13 @@
         <v>58</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>45001.677176620375</v>
       </c>
@@ -729,18 +790,23 @@
       <c r="M2" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="N2" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="O2" s="3" t="s">
         <v>77</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q2" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>89</v>
+      </c>
       <c r="R2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>45001.729072118054</v>
       </c>
@@ -780,13 +846,18 @@
       <c r="M3" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="N3" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="O3" s="3" t="s">
         <v>79</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q3" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="R3" s="1" t="s">
         <v>16</v>
       </c>
@@ -829,15 +900,20 @@
         <v>81</v>
       </c>
       <c r="M4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="P4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q4" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="5" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
@@ -877,20 +953,25 @@
         <v>91</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q5" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>96</v>
+      </c>
       <c r="R5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>45002.627384050924</v>
       </c>
@@ -928,20 +1009,25 @@
         <v>96</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q6" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="R6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>45002.650517083333</v>
       </c>
@@ -979,15 +1065,20 @@
         <v>86</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q7" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="R7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1736,6 +1827,17 @@
     <hyperlink ref="R2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="R7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="R12" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="Q2" r:id="rId4" location="/maplink/1" display="https://fr.wikipedia.org/wiki/La_Sauve - /maplink/1" xr:uid="{C6C9A15A-AB0F-4C06-A550-2465327E97F4}"/>
+    <hyperlink ref="N2" r:id="rId5" tooltip="Gironde (département)" display="https://fr.wikipedia.org/wiki/Gironde_(d%C3%A9partement)" xr:uid="{DE922D36-5B2C-4494-B018-C011115D7144}"/>
+    <hyperlink ref="N3" r:id="rId6" tooltip="Isère (département)" display="https://fr.wikipedia.org/wiki/Is%C3%A8re_(d%C3%A9partement)" xr:uid="{826151B7-3E68-4856-95CC-1424C9844A79}"/>
+    <hyperlink ref="Q3" r:id="rId7" location="/maplink/1" display="https://fr.wikipedia.org/wiki/Voiron - /maplink/1" xr:uid="{3E5C98D5-A111-4B50-A99A-9F284FC2FE33}"/>
+    <hyperlink ref="N4" r:id="rId8" tooltip="Ille-et-Vilaine" display="https://fr.wikipedia.org/wiki/Ille-et-Vilaine" xr:uid="{85258FE5-1D27-46DB-A22E-8B7D91DFF5E4}"/>
+    <hyperlink ref="Q4" r:id="rId9" location="/maplink/1" display="https://fr.wikipedia.org/wiki/Saint-Malo-de-Phily - /maplink/1" xr:uid="{E619C5AA-C1E4-410D-A58B-B411EDB7BF0C}"/>
+    <hyperlink ref="N5" r:id="rId10" tooltip="Meurthe-et-Moselle" display="https://fr.wikipedia.org/wiki/Meurthe-et-Moselle" xr:uid="{0C39027E-470B-4ED8-971A-4EBB36E3FE62}"/>
+    <hyperlink ref="Q5" r:id="rId11" location="/maplink/1" display="https://fr.wikipedia.org/wiki/Pompey - /maplink/1" xr:uid="{889F7680-8E2D-4B98-A5CA-90E41706493B}"/>
+    <hyperlink ref="N6" r:id="rId12" tooltip="Loire-Atlantique" display="https://fr.wikipedia.org/wiki/Loire-Atlantique" xr:uid="{6A12DA2C-1A5F-418F-89F8-EE42F1D22A80}"/>
+    <hyperlink ref="Q6" r:id="rId13" location="/maplink/1" display="https://fr.wikipedia.org/wiki/Nantes - /maplink/1" xr:uid="{4274F30A-A0C1-4390-A899-1B91C917BA25}"/>
+    <hyperlink ref="Q7" r:id="rId14" location="/maplink/1" display="https://fr.wikipedia.org/wiki/Dambach-la-Ville - /maplink/1" xr:uid="{D90FE50B-ECC4-4F17-B263-43DB5D634502}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>

</xml_diff>